<commit_message>
Ins Buffer Documentation Updates for ICD 2.5 (#383)
</commit_message>
<xml_diff>
--- a/docs/InsBufferFhirMappings.xlsx
+++ b/docs/InsBufferFhirMappings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhulbert/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhulbert/va/health-apis-vista-fhir-query/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DF5AAC-ED31-3A40-B911-05A1B76CE258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D22F960-50FD-284F-8B24-74DDE77A31EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{1868BA04-AF6E-6E4A-B504-822A4BD71A1E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="169">
   <si>
     <t>Field #</t>
   </si>
@@ -423,9 +423,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>.beneficiary.reference</t>
-  </si>
-  <si>
     <t>.beneficiary.identifier where type = MB</t>
   </si>
   <si>
@@ -462,9 +459,6 @@
     <t>payor.address</t>
   </si>
   <si>
-    <t>Contained Resource (Organization)</t>
-  </si>
-  <si>
     <t>.class.value(reference).identifier</t>
   </si>
   <si>
@@ -493,6 +487,60 @@
   </si>
   <si>
     <t>Patient/RelatedPerson</t>
+  </si>
+  <si>
+    <t>Static: 1 (YES)</t>
+  </si>
+  <si>
+    <t>.extension</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>See R4PatientTransformer for identifier system/code information</t>
+  </si>
+  <si>
+    <t>.beneficiary.generalPractitioner.name</t>
+  </si>
+  <si>
+    <t>.beneficiary.generalPractitioner.telecom</t>
+  </si>
+  <si>
+    <t>.beneficiary.identifier</t>
+  </si>
+  <si>
+    <t>.beneficiary</t>
+  </si>
+  <si>
+    <t>.name is a required field we won't populate for the insurance buffer file</t>
+  </si>
+  <si>
+    <t>.gender is a required field we won't populate for the insurance buffer file</t>
+  </si>
+  <si>
+    <t>Problems:</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Don't populate the .generalPractitioner field(s) and leave .beneficiary as a reference, not a contained resource</t>
+  </si>
+  <si>
+    <t>.subscriber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can RelatedPerson be used if the HIPAA relationship code is self? </t>
+  </si>
+  <si>
+    <t>Possible Solution</t>
+  </si>
+  <si>
+    <t>If yes, use RelatedPerson for the .subscriber field every time.</t>
   </si>
 </sst>
 </file>
@@ -877,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30A6421-B83D-6542-B4E9-697E7B35555D}">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -891,7 +939,7 @@
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -908,10 +956,10 @@
         <v>124</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>128</v>
@@ -931,13 +979,13 @@
         <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -954,13 +1002,13 @@
         <v>125</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -977,13 +1025,13 @@
         <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1000,13 +1048,13 @@
         <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1020,13 +1068,13 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1040,13 +1088,13 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -1061,13 +1109,13 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1081,13 +1129,13 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1101,13 +1149,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1121,13 +1169,13 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1141,13 +1189,13 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -1162,13 +1210,13 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G13" s="2"/>
     </row>
@@ -1186,13 +1234,13 @@
         <v>125</v>
       </c>
       <c r="E14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1206,13 +1254,13 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1226,13 +1274,13 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1246,13 +1294,13 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1266,13 +1314,13 @@
         <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1289,13 +1337,13 @@
         <v>125</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1312,10 +1360,10 @@
         <v>123</v>
       </c>
       <c r="E20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1332,10 +1380,10 @@
         <v>126</v>
       </c>
       <c r="E21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1352,10 +1400,10 @@
         <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1372,13 +1420,13 @@
         <v>126</v>
       </c>
       <c r="E23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>20.05</v>
       </c>
@@ -1389,12 +1437,14 @@
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E24" t="s">
-        <v>150</v>
-      </c>
-      <c r="F24" s="6"/>
+        <v>148</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
@@ -1410,10 +1460,10 @@
         <v>126</v>
       </c>
       <c r="E25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1430,10 +1480,10 @@
         <v>126</v>
       </c>
       <c r="E26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1450,10 +1500,10 @@
         <v>126</v>
       </c>
       <c r="E27" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1470,10 +1520,10 @@
         <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1490,10 +1540,10 @@
         <v>126</v>
       </c>
       <c r="E29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1510,13 +1560,13 @@
         <v>126</v>
       </c>
       <c r="E30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>40.01</v>
       </c>
@@ -1527,10 +1577,16 @@
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
+        <v>123</v>
+      </c>
+      <c r="E31" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="G31" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1544,10 +1600,7 @@
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>131</v>
-      </c>
-      <c r="G32" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1561,13 +1614,10 @@
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
-      </c>
-      <c r="G33" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>40.04</v>
       </c>
@@ -1578,13 +1628,16 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>131</v>
-      </c>
-      <c r="G34" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="E34" t="s">
+        <v>149</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>40.049999999999997</v>
       </c>
@@ -1595,13 +1648,16 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>131</v>
-      </c>
-      <c r="G35" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="E35" t="s">
+        <v>149</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>40.06</v>
       </c>
@@ -1612,13 +1668,16 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>131</v>
-      </c>
-      <c r="G36" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="E36" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>40.07</v>
       </c>
@@ -1629,13 +1688,16 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>131</v>
-      </c>
-      <c r="G37" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="E37" t="s">
+        <v>149</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>40.08</v>
       </c>
@@ -1646,10 +1708,13 @@
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>131</v>
-      </c>
-      <c r="G38" t="s">
-        <v>142</v>
+        <v>126</v>
+      </c>
+      <c r="E38" t="s">
+        <v>149</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1666,10 +1731,10 @@
         <v>126</v>
       </c>
       <c r="E39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1686,10 +1751,10 @@
         <v>126</v>
       </c>
       <c r="E40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F40" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1706,10 +1771,10 @@
         <v>126</v>
       </c>
       <c r="E41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F41" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1726,10 +1791,13 @@
         <v>123</v>
       </c>
       <c r="E42" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="F42" t="s">
-        <v>129</v>
+        <v>157</v>
+      </c>
+      <c r="G42" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1743,10 +1811,10 @@
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F43" t="s">
         <v>122</v>
@@ -1763,10 +1831,10 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F44" t="s">
         <v>118</v>
@@ -1783,7 +1851,7 @@
         <v>29</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1800,13 +1868,13 @@
         <v>125</v>
       </c>
       <c r="E46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G46" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1820,7 +1888,7 @@
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1834,7 +1902,7 @@
         <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1851,7 +1919,7 @@
         <v>123</v>
       </c>
       <c r="E49" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1865,13 +1933,13 @@
         <v>29</v>
       </c>
       <c r="D50" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E50" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>60.1</v>
       </c>
@@ -1882,10 +1950,16 @@
         <v>29</v>
       </c>
       <c r="D51" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="E51" t="s">
+        <v>153</v>
+      </c>
+      <c r="F51" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>60.11</v>
       </c>
@@ -1896,7 +1970,13 @@
         <v>29</v>
       </c>
       <c r="D52" t="s">
-        <v>131</v>
+        <v>126</v>
+      </c>
+      <c r="E52" t="s">
+        <v>153</v>
+      </c>
+      <c r="F52" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1910,10 +1990,10 @@
         <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F53" t="s">
         <v>117</v>
@@ -1930,10 +2010,10 @@
         <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E54" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1950,13 +2030,13 @@
         <v>123</v>
       </c>
       <c r="E55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F55" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>60.15</v>
       </c>
@@ -1967,10 +2047,13 @@
         <v>69</v>
       </c>
       <c r="D56" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="F56" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>60.16</v>
       </c>
@@ -1981,7 +2064,10 @@
         <v>29</v>
       </c>
       <c r="D57" t="s">
-        <v>131</v>
+        <v>126</v>
+      </c>
+      <c r="E57" t="s">
+        <v>135</v>
       </c>
       <c r="F57" t="s">
         <v>120</v>
@@ -1998,7 +2084,7 @@
         <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2012,7 +2098,7 @@
         <v>29</v>
       </c>
       <c r="D59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2026,7 +2112,7 @@
         <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2040,7 +2126,7 @@
         <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2054,7 +2140,7 @@
         <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2068,7 +2154,7 @@
         <v>29</v>
       </c>
       <c r="D63" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2082,7 +2168,7 @@
         <v>29</v>
       </c>
       <c r="D64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2096,7 +2182,7 @@
         <v>29</v>
       </c>
       <c r="D65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2110,7 +2196,7 @@
         <v>29</v>
       </c>
       <c r="D66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2124,7 +2210,7 @@
         <v>39</v>
       </c>
       <c r="D67" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2138,7 +2224,7 @@
         <v>29</v>
       </c>
       <c r="D68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2152,7 +2238,7 @@
         <v>29</v>
       </c>
       <c r="D69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2169,10 +2255,10 @@
         <v>123</v>
       </c>
       <c r="E70" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="F70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2189,7 +2275,7 @@
         <v>126</v>
       </c>
       <c r="E71" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2206,7 +2292,7 @@
         <v>126</v>
       </c>
       <c r="E72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2223,7 +2309,7 @@
         <v>126</v>
       </c>
       <c r="E73" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2240,7 +2326,7 @@
         <v>126</v>
       </c>
       <c r="E74" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2257,7 +2343,7 @@
         <v>126</v>
       </c>
       <c r="E75" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2274,7 +2360,7 @@
         <v>126</v>
       </c>
       <c r="E76" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2291,7 +2377,7 @@
         <v>126</v>
       </c>
       <c r="E77" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2308,7 +2394,7 @@
         <v>126</v>
       </c>
       <c r="E78" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2325,7 +2411,7 @@
         <v>123</v>
       </c>
       <c r="E79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F79" t="s">
         <v>127</v>
@@ -2342,7 +2428,7 @@
         <v>93</v>
       </c>
       <c r="D80" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2356,7 +2442,7 @@
         <v>93</v>
       </c>
       <c r="D81" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2370,7 +2456,7 @@
         <v>93</v>
       </c>
       <c r="D82" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2384,7 +2470,7 @@
         <v>93</v>
       </c>
       <c r="D83" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2398,7 +2484,7 @@
         <v>93</v>
       </c>
       <c r="D84" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2412,7 +2498,7 @@
         <v>93</v>
       </c>
       <c r="D85" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2426,7 +2512,7 @@
         <v>93</v>
       </c>
       <c r="D86" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2440,7 +2526,7 @@
         <v>93</v>
       </c>
       <c r="D87" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2454,7 +2540,7 @@
         <v>93</v>
       </c>
       <c r="D88" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2468,7 +2554,7 @@
         <v>93</v>
       </c>
       <c r="D89" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2482,7 +2568,7 @@
         <v>93</v>
       </c>
       <c r="D90" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2496,7 +2582,7 @@
         <v>93</v>
       </c>
       <c r="D91" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2510,7 +2596,7 @@
         <v>93</v>
       </c>
       <c r="D92" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2524,7 +2610,7 @@
         <v>93</v>
       </c>
       <c r="D93" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2538,7 +2624,7 @@
         <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2552,7 +2638,7 @@
         <v>93</v>
       </c>
       <c r="D95" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2566,7 +2652,7 @@
         <v>93</v>
       </c>
       <c r="D96" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2580,7 +2666,7 @@
         <v>93</v>
       </c>
       <c r="D97" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2594,7 +2680,7 @@
         <v>93</v>
       </c>
       <c r="D98" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -2611,10 +2697,10 @@
         <v>126</v>
       </c>
       <c r="E99" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F99" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -2628,13 +2714,13 @@
         <v>29</v>
       </c>
       <c r="D100" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E100" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F100" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -2651,7 +2737,7 @@
         <v>123</v>
       </c>
       <c r="E101" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F101" t="s">
         <v>121</v>
@@ -2671,7 +2757,57 @@
         <v>123</v>
       </c>
       <c r="E102" t="s">
-        <v>152</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B105" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D105" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B106" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C107" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D107" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C108" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D108" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B109" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C110" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D110" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved mappings and example for Coverage writes to buffer file(#386)
</commit_message>
<xml_diff>
--- a/docs/InsBufferFhirMappings.xlsx
+++ b/docs/InsBufferFhirMappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhulbert/va/health-apis-vista-fhir-query/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D22F960-50FD-284F-8B24-74DDE77A31EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BF3F9D-99D5-4546-8E91-75471EFAF4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{1868BA04-AF6E-6E4A-B504-822A4BD71A1E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="176">
   <si>
     <t>Field #</t>
   </si>
@@ -486,9 +486,6 @@
     <t>InsurancePlan</t>
   </si>
   <si>
-    <t>Patient/RelatedPerson</t>
-  </si>
-  <si>
     <t>Static: 1 (YES)</t>
   </si>
   <si>
@@ -498,9 +495,6 @@
     <t>Patient</t>
   </si>
   <si>
-    <t>See R4PatientTransformer for identifier system/code information</t>
-  </si>
-  <si>
     <t>.beneficiary.generalPractitioner.name</t>
   </si>
   <si>
@@ -541,6 +535,33 @@
   </si>
   <si>
     <t>If yes, use RelatedPerson for the .subscriber field every time.</t>
+  </si>
+  <si>
+    <t>RelatedPerson</t>
+  </si>
+  <si>
+    <t>.birthDate</t>
+  </si>
+  <si>
+    <t>.identifier</t>
+  </si>
+  <si>
+    <t>See R4PatientTransformer for identifier system/code details: https://github.com/department-of-veterans-affairs/health-apis-data-query/blob/a6b5bb26a88606753fdfff227cd23f4e918b08b9/data-query/src/main/java/gov/va/api/health/dataquery/service/controller/patient/R4PatientTransformer.java#L417</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/STU4/StructureDefinition-us-core-birthsex.html</t>
+  </si>
+  <si>
+    <t>See R4PatientTransformer for identifier system/code details: https://github.com/department-of-veterans-affairs/health-apis-data-query/blob/a6b5bb26a88606753fdfff227cd23f4e918b08b9/data-query/src/main/java/gov/va/api/health/dataquery/service/controller/patient/R4PatientTransformer.java#L399</t>
+  </si>
+  <si>
+    <t>.address</t>
+  </si>
+  <si>
+    <t>.telecom</t>
+  </si>
+  <si>
+    <t>.name.text</t>
   </si>
 </sst>
 </file>
@@ -927,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30A6421-B83D-6542-B4E9-697E7B35555D}">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -939,7 +960,7 @@
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1443,7 +1464,7 @@
         <v>148</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1586,7 +1607,7 @@
         <v>135</v>
       </c>
       <c r="G31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -1634,7 +1655,7 @@
         <v>149</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1654,7 +1675,7 @@
         <v>149</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1674,7 +1695,7 @@
         <v>149</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1694,7 +1715,7 @@
         <v>149</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1714,7 +1735,7 @@
         <v>149</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1791,13 +1812,13 @@
         <v>123</v>
       </c>
       <c r="E42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F42" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G42" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1905,7 +1926,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>60.08</v>
       </c>
@@ -1919,10 +1940,13 @@
         <v>123</v>
       </c>
       <c r="E49" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="F49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>60.09</v>
       </c>
@@ -1936,10 +1960,16 @@
         <v>126</v>
       </c>
       <c r="E50" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="F50" t="s">
+        <v>169</v>
+      </c>
+      <c r="G50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>60.1</v>
       </c>
@@ -1953,13 +1983,13 @@
         <v>126</v>
       </c>
       <c r="E51" t="s">
+        <v>152</v>
+      </c>
+      <c r="F51" t="s">
         <v>153</v>
       </c>
-      <c r="F51" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>60.11</v>
       </c>
@@ -1973,13 +2003,13 @@
         <v>126</v>
       </c>
       <c r="E52" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F52" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>60.12</v>
       </c>
@@ -1999,7 +2029,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>60.13</v>
       </c>
@@ -2013,10 +2043,16 @@
         <v>126</v>
       </c>
       <c r="E54" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="F54" t="s">
+        <v>151</v>
+      </c>
+      <c r="G54" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>60.14</v>
       </c>
@@ -2036,7 +2072,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>60.15</v>
       </c>
@@ -2053,7 +2089,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>60.16</v>
       </c>
@@ -2073,7 +2109,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>61.01</v>
       </c>
@@ -2087,7 +2123,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>61.02</v>
       </c>
@@ -2101,7 +2137,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>61.03</v>
       </c>
@@ -2115,7 +2151,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>61.04</v>
       </c>
@@ -2129,7 +2165,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>61.05</v>
       </c>
@@ -2143,7 +2179,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>61.06</v>
       </c>
@@ -2157,7 +2193,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>61.07</v>
       </c>
@@ -2255,7 +2291,7 @@
         <v>123</v>
       </c>
       <c r="E70" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F70" t="s">
         <v>129</v>
@@ -2275,7 +2311,10 @@
         <v>126</v>
       </c>
       <c r="E71" t="s">
-        <v>150</v>
+        <v>167</v>
+      </c>
+      <c r="F71" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2292,7 +2331,10 @@
         <v>126</v>
       </c>
       <c r="E72" t="s">
-        <v>150</v>
+        <v>167</v>
+      </c>
+      <c r="F72" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2309,7 +2351,10 @@
         <v>126</v>
       </c>
       <c r="E73" t="s">
-        <v>150</v>
+        <v>167</v>
+      </c>
+      <c r="F73" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2326,7 +2371,10 @@
         <v>126</v>
       </c>
       <c r="E74" t="s">
-        <v>150</v>
+        <v>167</v>
+      </c>
+      <c r="F74" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2343,7 +2391,10 @@
         <v>126</v>
       </c>
       <c r="E75" t="s">
-        <v>150</v>
+        <v>167</v>
+      </c>
+      <c r="F75" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2360,7 +2411,10 @@
         <v>126</v>
       </c>
       <c r="E76" t="s">
-        <v>150</v>
+        <v>167</v>
+      </c>
+      <c r="F76" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2377,7 +2431,10 @@
         <v>126</v>
       </c>
       <c r="E77" t="s">
-        <v>150</v>
+        <v>167</v>
+      </c>
+      <c r="F77" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2394,7 +2451,10 @@
         <v>126</v>
       </c>
       <c r="E78" t="s">
-        <v>150</v>
+        <v>167</v>
+      </c>
+      <c r="F78" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2757,57 +2817,60 @@
         <v>123</v>
       </c>
       <c r="E102" t="s">
-        <v>150</v>
+        <v>167</v>
+      </c>
+      <c r="F102" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B105" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D105" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B106" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C107" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D107" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C108" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D108" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B109" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C110" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D110" t="s">
         <v>166</v>
-      </c>
-      <c r="D110" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Docs: Service Date is required field (#450)
</commit_message>
<xml_diff>
--- a/docs/InsBufferFhirMappings.xlsx
+++ b/docs/InsBufferFhirMappings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhulbert/va/health-apis-vista-fhir-query/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9840322C-9465-1C43-9DFF-32463C61574E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE61973A-CC46-D742-973F-FD1EC56A7352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{1868BA04-AF6E-6E4A-B504-822A4BD71A1E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="166">
   <si>
     <t>Field #</t>
   </si>
@@ -504,39 +504,6 @@
     <t>.beneficiary.identifier</t>
   </si>
   <si>
-    <t>.beneficiary</t>
-  </si>
-  <si>
-    <t>.name is a required field we won't populate for the insurance buffer file</t>
-  </si>
-  <si>
-    <t>.gender is a required field we won't populate for the insurance buffer file</t>
-  </si>
-  <si>
-    <t>Problems:</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>Problem</t>
-  </si>
-  <si>
-    <t>Don't populate the .generalPractitioner field(s) and leave .beneficiary as a reference, not a contained resource</t>
-  </si>
-  <si>
-    <t>.subscriber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can RelatedPerson be used if the HIPAA relationship code is self? </t>
-  </si>
-  <si>
-    <t>Possible Solution</t>
-  </si>
-  <si>
-    <t>If yes, use RelatedPerson for the .subscriber field every time.</t>
-  </si>
-  <si>
     <t>RelatedPerson</t>
   </si>
   <si>
@@ -564,10 +531,7 @@
     <t>.name.text</t>
   </si>
   <si>
-    <t>.payor.active</t>
-  </si>
-  <si>
-    <t>Active flag is required by Carin BB Organization, but insurance buffer does not have a corresponding field.</t>
+    <t>If not provided, default to today</t>
   </si>
 </sst>
 </file>
@@ -952,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30A6421-B83D-6542-B4E9-697E7B35555D}">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1361,16 +1325,16 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E19" t="s">
         <v>135</v>
       </c>
       <c r="F19" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1824,7 +1788,7 @@
         <v>155</v>
       </c>
       <c r="G42" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1946,10 +1910,10 @@
         <v>123</v>
       </c>
       <c r="E49" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F49" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1966,13 +1930,13 @@
         <v>126</v>
       </c>
       <c r="E50" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F50" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="G50" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -2049,13 +2013,13 @@
         <v>126</v>
       </c>
       <c r="E54" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F54" t="s">
         <v>151</v>
       </c>
       <c r="G54" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -2317,10 +2281,10 @@
         <v>126</v>
       </c>
       <c r="E71" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F71" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2337,10 +2301,10 @@
         <v>126</v>
       </c>
       <c r="E72" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F72" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2357,10 +2321,10 @@
         <v>126</v>
       </c>
       <c r="E73" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F73" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2377,10 +2341,10 @@
         <v>126</v>
       </c>
       <c r="E74" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F74" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2397,10 +2361,10 @@
         <v>126</v>
       </c>
       <c r="E75" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F75" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2417,10 +2381,10 @@
         <v>126</v>
       </c>
       <c r="E76" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F76" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2437,10 +2401,10 @@
         <v>126</v>
       </c>
       <c r="E77" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F77" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2457,10 +2421,10 @@
         <v>126</v>
       </c>
       <c r="E78" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F78" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2823,68 +2787,10 @@
         <v>123</v>
       </c>
       <c r="E102" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F102" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B105" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D105" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B106" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C107" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D107" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C108" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D108" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B109" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C110" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="D110" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B111" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>